<commit_message>
Test-4 results for thisyear
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-4.xlsx
+++ b/migforecasting/underground/test-4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates test (Next Year)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t>test size 20%</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>С координатами</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-2.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-Cor-2.csv) - this year</t>
   </si>
 </sst>
 </file>
@@ -2435,8 +2441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:U67"/>
   <sheetViews>
-    <sheetView topLeftCell="F61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y64" sqref="Y64"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U62" sqref="U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4569,14 +4575,1201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.2056791044918189</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.2729879855922368</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.99010581731100722</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4.755437464936823</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.99795762614404582</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.3400541455661759</v>
+      </c>
+      <c r="H6" s="2">
+        <f>H5+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.144880873572927</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.367463151464217</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.13311698930376</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4.4462560975719221</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H54" si="1">H6+1</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.99887386398141031</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.727049170634253</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.125196249673893</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3.047146786999464</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.1841233464631</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3.972890143371552</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.94034876774283982</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5.3256141378915798</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.1424852275997459</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.484757122422943</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.0121474857262169</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.0935257716333666</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.89706182683278102</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.9236517018926311</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.0215708125950289</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4.6239216862370558</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.3003259094846811</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.702587980664297</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.138917364969726</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3.9544372342178828</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.3295667134781419</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.6944659023184701</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.0570581444786731</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2.5812904422824481</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.2450310982905599</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.4510527456154421</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.2117980735284719</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.677596723500917</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.078073056050775</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2.6087313263381109</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.5252678619409561</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2.0949053100808008</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.304037725809188</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1.871510240216953</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.1896217616969209</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2.2609062125685142</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1.0993167124124981</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.5624874748073869</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.3086360885859349</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.851207611589089</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1.225109552911682</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2.2693719483593591</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.077026451559286</v>
+      </c>
+      <c r="E18" s="3">
+        <v>4.1530368143786029</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.80493404628916332</v>
+      </c>
+      <c r="J18" s="3">
+        <v>5.7700277768434143</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.356206693529314</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1.839396885268415</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1.283833389394101</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2.745956757258071</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.1900963614755851</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2.187063856021787</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.249925299001339</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2.8258904537562959</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.08526160831916</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.60004595633669</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1.2835962950171469</v>
+      </c>
+      <c r="J21" s="3">
+        <v>3.1492865994721631</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.98063972528183418</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4.0375333828575197</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1.1651783331484931</v>
+      </c>
+      <c r="J22" s="3">
+        <v>4.0902302936364574</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1.247853113988759</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1.7883271602324831</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1.2448808449132129</v>
+      </c>
+      <c r="J23" s="3">
+        <v>2.2964856644062461</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.3026846083723591</v>
+      </c>
+      <c r="E24" s="3">
+        <v>2.7567520245772501</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.77840755635677739</v>
+      </c>
+      <c r="J24" s="3">
+        <v>6.4030476708896158</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1.099241135447669</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2.4795267418455089</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1.11414643697085</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2.3769388103483942</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.285968036394874</v>
+      </c>
+      <c r="E26" s="3">
+        <v>3.121608480448121</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.85168930971484302</v>
+      </c>
+      <c r="J26" s="3">
+        <v>4.8025543640262844</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1.1904958824152601</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2.2181372187220778</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1.1426937797762879</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2.7301351688435038</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.8998473243361742</v>
+      </c>
+      <c r="E28" s="3">
+        <v>7.09467169486771</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1.164482520509071</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3.3442202553686782</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1.468253258723812</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2.0598754398207682</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.1482151837829819</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1.847075495220708</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1.2405468639603969</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2.2424909217316151</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1.1253308824249011</v>
+      </c>
+      <c r="J30" s="3">
+        <v>3.328469988157674</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.320821067296722</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.608599231783272</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.91764883079866333</v>
+      </c>
+      <c r="J31" s="3">
+        <v>4.9862867123982806</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1.2043568008466421</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2.328319183134639</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="3">
+        <v>1.537572795317284</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2.4870072681934738</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1.1481534644030471</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1.9602978792595189</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1.2252261351552121</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2.718034784340202</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.191427924979201</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2.886479600721982</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1.388310536769217</v>
+      </c>
+      <c r="J34" s="3">
+        <v>1.8289079966518149</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1.397398083734074</v>
+      </c>
+      <c r="E35" s="3">
+        <v>2.0370402508698948</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.064643667599652</v>
+      </c>
+      <c r="J35" s="3">
+        <v>3.8717355010166221</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.063087104993955</v>
+      </c>
+      <c r="E36" s="3">
+        <v>2.7495281753048468</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1.198919743095205</v>
+      </c>
+      <c r="J36" s="3">
+        <v>3.5089165140923608</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.208349551353872</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2.560692724154114</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.164633594240416</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2.4443536793977798</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1.0376609122206899</v>
+      </c>
+      <c r="E38" s="3">
+        <v>3.5619617170987632</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1.201318399014351</v>
+      </c>
+      <c r="J38" s="3">
+        <v>3.9772174439170218</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1.347269213052021</v>
+      </c>
+      <c r="E39" s="3">
+        <v>2.4589019659816072</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0.92372121232995974</v>
+      </c>
+      <c r="J39" s="3">
+        <v>4.3176631117326254</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1.08397405059351</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1.867224051310461</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1.0314559449174421</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1.6119337139459371</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1.1673806908197391</v>
+      </c>
+      <c r="E41" s="3">
+        <v>2.16408464525334</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1.182961295771686</v>
+      </c>
+      <c r="J41" s="3">
+        <v>1.7731368831084811</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1.1131675225327931</v>
+      </c>
+      <c r="E42" s="3">
+        <v>3.0341103181973459</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1.1501279829137141</v>
+      </c>
+      <c r="J42" s="3">
+        <v>2.3370419548684018</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1.317787310340967</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1.9015016274806491</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.0622991282835439</v>
+      </c>
+      <c r="J43" s="3">
+        <v>3.5054549940160542</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.85357227491798637</v>
+      </c>
+      <c r="E44" s="3">
+        <v>6.7284237569665981</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1.3104638061468921</v>
+      </c>
+      <c r="J44" s="3">
+        <v>2.01290303377997</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1.2667193803499599</v>
+      </c>
+      <c r="E45" s="3">
+        <v>2.5562570431765161</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1.0834164223612559</v>
+      </c>
+      <c r="J45" s="3">
+        <v>2.943680898501877</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1.2665557089188391</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2.3333529682993772</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0.98321771299276162</v>
+      </c>
+      <c r="J46" s="3">
+        <v>5.0889663271109402</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.1362498679997659</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2.5732707697016921</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1.1456130289731279</v>
+      </c>
+      <c r="J47" s="3">
+        <v>4.3223304044727344</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1.043925586311016</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2.9588101316047331</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1.5301318996244979</v>
+      </c>
+      <c r="J48" s="3">
+        <v>1.5127853054604681</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1.1640722779636701</v>
+      </c>
+      <c r="E49" s="3">
+        <v>3.1516746441330592</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1.08557747581812</v>
+      </c>
+      <c r="J49" s="3">
+        <v>4.510827394320855</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1.12677083333433</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1.876406953901137</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1.3405868349321399</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2.958046043122232</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.88592487970189449</v>
+      </c>
+      <c r="E51" s="3">
+        <v>6.5971396548057202</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1.215777140123407</v>
+      </c>
+      <c r="J51" s="3">
+        <v>1.824662786665967</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1.1628513982455959</v>
+      </c>
+      <c r="E52" s="3">
+        <v>2.263982885489348</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1.3375957099542459</v>
+      </c>
+      <c r="J52" s="3">
+        <v>2.069577828507942</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1.3763428007271949</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.3741232428182348</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1.1368957409110201</v>
+      </c>
+      <c r="J53" s="3">
+        <v>3.0154392046166301</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1.274361759814852</v>
+      </c>
+      <c r="E54" s="3">
+        <v>2.9399033213789258</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0.98943852147910616</v>
+      </c>
+      <c r="J54" s="3">
+        <v>4.2970362442436949</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="3">
+        <f>AVERAGE(D5:D54)</f>
+        <v>1.1689923572027021</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>2.9724080693133152</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I56" s="3">
+        <f>AVERAGE(I5:I54)</f>
+        <v>1.1500771832204117</v>
+      </c>
+      <c r="J56" s="3">
+        <f>AVERAGE(J5:J54)</f>
+        <v>3.0605144339950447</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>0.14528175160352255</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>1.3111645875663389</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I57" s="3">
+        <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>0.16159688826316657</v>
+      </c>
+      <c r="J57" s="3">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>1.2028298560385329</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New test results (fed. dist.)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-4.xlsx
+++ b/migforecasting/underground/test-4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates test (Next Year)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="18">
   <si>
     <t>test size 20%</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>NN(64,64,64,64,1) (citiesdataset-NY-2.csv) - next year</t>
+  </si>
+  <si>
+    <t>NN(64,64,64,64,1) (citiesdataset-NYCor-2.csv) - next year</t>
   </si>
 </sst>
 </file>
@@ -2450,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AG67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD31" sqref="AD31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,7 +2514,7 @@
         <v>16</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="3:33" x14ac:dyDescent="0.25">
@@ -5024,7 +5027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J57"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>

</xml_diff>